<commit_message>
fixed manual guessing of frequency
</commit_message>
<xml_diff>
--- a/Sinusoidal level 4 spreadsheet.xlsx
+++ b/Sinusoidal level 4 spreadsheet.xlsx
@@ -13,17 +13,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Sinusoidal parent function</t>
+    <t>Tide height (ft) x hours after jan 1 12 am</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -47,11 +53,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -276,51 +285,163 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.0</v>
+      <c r="A2" s="2">
+        <v>5.85</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-0.05</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.84147098</v>
+      <c r="A3" s="2">
+        <v>11.82</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.19</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.90929743</v>
+      <c r="A4" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.61</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.14112001</v>
+      <c r="A5" s="2">
+        <v>24.35</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7.39</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>-0.7568025</v>
+      <c r="A6" s="2">
+        <v>30.58</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-0.17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>-0.95892427</v>
+      <c r="A7" s="2">
+        <v>36.55</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8.18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>43.17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>49.07</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>55.37</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>61.33</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8.05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>67.88</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-0.62</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>73.83</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>80.2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>86.17</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>92.67</v>
+      </c>
+      <c r="B16" s="2">
+        <v>-0.51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>98.65</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>104.15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>110.05</v>
+      </c>
+      <c r="B19" s="2">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>116.52</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-0.33</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>122.53</v>
+      </c>
+      <c r="B21" s="2">
+        <v>7.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>